<commit_message>
makr var3or4argfunction support array formulas
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/TestArrayAggregations.xlsx
+++ b/test-data/spreadsheet/TestArrayAggregations.xlsx
@@ -481,13 +481,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F18" sqref="F18:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -815,9 +820,15 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F18">
-        <f t="array" ref="F18">SUM(D2:D17+F2:F17+A2:A17)</f>
-        <v>189827</v>
+      <c r="F18" t="e">
+        <f>SUBSTITUTE(F2:F17,"0","Do",1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="array" ref="F19">SUBSTITUTE(F3:F18,"10","Do",1)</f>
+        <v>7200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduce new methods to the Function
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/TestArrayAggregations.xlsx
+++ b/test-data/spreadsheet/TestArrayAggregations.xlsx
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:F19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
     <col min="10" max="10" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -534,8 +534,11 @@
         <f t="array" ref="F2:F17">D2:D17*E2:E17</f>
         <v>10500</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -552,8 +555,11 @@
       <c r="F3" s="5">
         <v>7200</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -572,8 +578,11 @@
       <c r="F4" s="2">
         <v>13800</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -590,8 +599,11 @@
       <c r="F5" s="5">
         <v>13600</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -610,8 +622,11 @@
       <c r="F6" s="2">
         <v>6000</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -628,8 +643,11 @@
       <c r="F7" s="5">
         <v>1600</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -648,8 +666,11 @@
       <c r="F8" s="2">
         <v>19350</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -666,8 +687,11 @@
       <c r="F9" s="5">
         <v>9750</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -686,8 +710,11 @@
       <c r="F10" s="2">
         <v>13500</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -704,8 +731,11 @@
       <c r="F11" s="5">
         <v>16000</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -724,8 +754,11 @@
       <c r="F12" s="6">
         <v>15000</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -742,8 +775,11 @@
       <c r="F13" s="2">
         <v>13300</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -762,8 +798,11 @@
       <c r="F14" s="5">
         <v>8800</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -780,8 +819,11 @@
       <c r="F15" s="2">
         <v>6000</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -800,8 +842,11 @@
       <c r="F16" s="5">
         <v>18400</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -818,17 +863,24 @@
       <c r="F17" s="2">
         <v>16800</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F18" t="e">
-        <f>SUBSTITUTE(F2:F17,"0","Do",1)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F19" t="str">
-        <f t="array" ref="F19">SUBSTITUTE(F3:F18,"10","Do",1)</f>
-        <v>7200</v>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <f>D18:D33*E18:E33</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="array" ref="G18">SUM({1,2,3;1,2,3;1,2,3})</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="array" ref="F19">MATCH(13300,F2:F17,0)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix cross sheet ranges
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/TestArrayAggregations.xlsx
+++ b/test-data/spreadsheet/TestArrayAggregations.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="435" windowWidth="24675" windowHeight="10770"/>
+    <workbookView xWindow="360" yWindow="435" windowWidth="24675" windowHeight="10770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,6 +878,18 @@
         <v>42020</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="array" ref="F18">COUNTIFS(C2,"Coupe",D2,8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="array" ref="A20">SUM(A2:A17)</f>
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -885,81 +897,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F18:N28"/>
+  <dimension ref="A2:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F18">
-        <f>COLUMN(A2:F17)</f>
+    <row r="2" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F21">
-        <f t="array" ref="F21:F28">COLUMN(A2:F17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <f t="array" ref="H22:N22">COLUMN(A2:F17)</f>
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
+    <row r="8" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>3</v>
       </c>
-      <c r="K22">
-        <v>4</v>
-      </c>
-      <c r="L22">
-        <v>5</v>
-      </c>
-      <c r="M22">
-        <v>6</v>
-      </c>
-      <c r="N22" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F28">
-        <v>1</v>
+    </row>
+    <row r="16" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>